<commit_message>
Final commit for Recipe scraping
</commit_message>
<xml_diff>
--- a/Team02_NinjaScrapers_2023/src/test/resources/IngredientsForDiabetes.xlsx
+++ b/Team02_NinjaScrapers_2023/src/test/resources/IngredientsForDiabetes.xlsx
@@ -3,16 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{CD03F1BF-0395-4D8D-94B1-FA662247008C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akash\git\RecipeScrapingHackathon2023\Team02_NinjaScrapers_2023\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ED95B8D-555D-401F-9D9D-F99472D748DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{38CB68C0-1252-4FCE-B843-91052F49BB13}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{38CB68C0-1252-4FCE-B843-91052F49BB13}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:E12"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>Sugar</t>
   </si>
@@ -310,13 +316,58 @@
   </si>
   <si>
     <t>Mushrooms</t>
+  </si>
+  <si>
+    <t>Allergies</t>
+  </si>
+  <si>
+    <t>milk</t>
+  </si>
+  <si>
+    <t>soy</t>
+  </si>
+  <si>
+    <t>egg</t>
+  </si>
+  <si>
+    <t>sesame</t>
+  </si>
+  <si>
+    <t>shellfish</t>
+  </si>
+  <si>
+    <t>seafood</t>
+  </si>
+  <si>
+    <t>Nut Allergies</t>
+  </si>
+  <si>
+    <t>peanuts</t>
+  </si>
+  <si>
+    <t>walnuts</t>
+  </si>
+  <si>
+    <t>almond</t>
+  </si>
+  <si>
+    <t>hazelnut</t>
+  </si>
+  <si>
+    <t>cashew</t>
+  </si>
+  <si>
+    <t>pecan</t>
+  </si>
+  <si>
+    <t>pistachio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +409,14 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -431,10 +490,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1136,7 +1193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{088F14A3-3EC3-4E74-BAF5-C0FC8F0C74E1}">
   <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1151,113 +1208,218 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="3" t="s">
         <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A954BBAC-1A85-43CD-963A-F7D52892BCBF}">
+  <dimension ref="A1:A7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F12E784-C7DD-43F7-97C3-726B92A1AD40}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>